<commit_message>
updated datastructures module related pages
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/Excel_Register_Login_Pythoncode_Practice.xlsx
+++ b/src/test/resources/testData/Excel_Register_Login_Pythoncode_Practice.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\geeta\eclipse-workspace-2023\TestNG\Dsalgo_TestNG_Project\src\test\resources\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A43B92DF-D2EF-427F-BB6C-1DBFD32D2513}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8109333E-C413-4996-A0CA-BA60E175F721}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3900" yWindow="3900" windowWidth="21600" windowHeight="12645" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" firstSheet="3" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Invalid_LogIn2" sheetId="1" r:id="rId1"/>
@@ -20,18 +20,21 @@
     <sheet name="pythonCodeold" sheetId="2" r:id="rId5"/>
     <sheet name="pythonCode" sheetId="7" r:id="rId6"/>
     <sheet name="ArrayTopicCode" sheetId="9" r:id="rId7"/>
+    <sheet name="DsTimeComplexityold" sheetId="10" r:id="rId8"/>
+    <sheet name="DsTimeComplexityValid" sheetId="11" r:id="rId9"/>
+    <sheet name="DsTimeComplexityInvalid" sheetId="12" r:id="rId10"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId8" roundtripDataChecksum="EtCkI7veSjd8xyGA1meF/qbOwVoJNm+1VkhWI1ll20o="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId11" roundtripDataChecksum="EtCkI7veSjd8xyGA1meF/qbOwVoJNm+1VkhWI1ll20o="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="68">
   <si>
     <t>username</t>
   </si>
@@ -288,16 +291,35 @@
   <si>
     <t>Code</t>
   </si>
+  <si>
+    <t>Time Complexity</t>
+  </si>
+  <si>
+    <t>https://dsportalapp.herokuapp.com/tryEditor</t>
+  </si>
+  <si>
+    <t>Invalid</t>
+  </si>
+  <si>
+    <t>Invalid Code</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -335,6 +357,13 @@
       <name val="Courier New"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -369,22 +398,27 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1673,6 +1707,49 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE6A027C-407B-4D40-A7A6-3466D906A522}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="C2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>65</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -3160,8 +3237,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7B7D2B-12A7-458E-9193-737F567EB08C}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3224,4 +3301,113 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE4A347B-513F-49DD-A850-7AA5FD4A4C3E}">
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{881EAAD1-E8E5-4C86-AEF5-33626AAF4B27}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>65</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>